<commit_message>
boat web site scrap
</commit_message>
<xml_diff>
--- a/IMDB/Top Rated Movies.xlsx
+++ b/IMDB/Top Rated Movies.xlsx
@@ -5159,12 +5159,12 @@
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Stand by Me</t>
+          <t>The Terminator</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>1986</t>
+          <t>1984</t>
         </is>
       </c>
       <c r="D216" t="inlineStr">
@@ -5181,12 +5181,12 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>The Terminator</t>
+          <t>Stand by Me</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>1984</t>
+          <t>1986</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">

</xml_diff>